<commit_message>
Agregado de productos en la planilla de cuenta 3 para subir a meli
</commit_message>
<xml_diff>
--- a/migracionWordPressPrestashop/Listado de Productos con combinaciones filtrados.xlsx
+++ b/migracionWordPressPrestashop/Listado de Productos con combinaciones filtrados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archivos_bat\archivos_bat\migracionWordPressPrestashop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$BE$461</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -6672,8 +6675,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -6701,8 +6712,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6985,180 +6997,186 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE461"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:BE1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>2213</v>
       </c>
     </row>
@@ -61579,6 +61597,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:BE461"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>